<commit_message>
Initial commit to GitHub
</commit_message>
<xml_diff>
--- a/PartsAndVoltages.xlsx
+++ b/PartsAndVoltages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="12465"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19035" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Part Selection" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -387,10 +388,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -715,7 +716,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L66" sqref="L66"/>
+      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,39 +790,39 @@
       <c r="O2" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="36"/>
-      <c r="AJ2" s="36"/>
-      <c r="AK2" s="36"/>
-      <c r="AL2" s="36"/>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="36"/>
-      <c r="AO2" s="36"/>
-      <c r="AP2" s="36"/>
-      <c r="AQ2" s="36"/>
-      <c r="AR2" s="36"/>
-      <c r="AS2" s="36"/>
-      <c r="AT2" s="36"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
     </row>
     <row r="3" spans="1:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G3" s="24"/>
@@ -1040,11 +1041,11 @@
       <c r="C7" s="18">
         <v>10.59</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <f>IF(B7&lt;&gt;0,B7*C7,"")</f>
         <v>10.59</v>
       </c>
-      <c r="E7" s="19" t="str">
+      <c r="E7" s="20" t="str">
         <f>HYPERLINK("http://www.digikey.ca/product-detail/en/OVM7690-R20A/884-1019-1-ND/","OVM7690-R20A")</f>
         <v>OVM7690-R20A</v>
       </c>
@@ -1117,7 +1118,7 @@
     <row r="8" spans="1:47" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="37" t="str">
+      <c r="D8" s="36" t="str">
         <f t="shared" ref="D8:D48" si="1">IF(B8&lt;&gt;0,B8*C8,"")</f>
         <v/>
       </c>
@@ -1352,15 +1353,17 @@
       <c r="AU11" s="2"/>
     </row>
     <row r="12" spans="1:47" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
       <c r="C12" s="18">
         <v>16.71</v>
       </c>
-      <c r="D12" s="37" t="str">
+      <c r="D12" s="36">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E12" s="19" t="str">
+        <v>16.71</v>
+      </c>
+      <c r="E12" s="20" t="str">
         <f>HYPERLINK("http://www.digikey.ca/product-detail/en/MAX5851ETL%2B/MAX5851ETL%2B-ND","MAX5851ETL+")</f>
         <v>MAX5851ETL+</v>
       </c>
@@ -1368,27 +1371,31 @@
         <v>20</v>
       </c>
       <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K12" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="L12" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+      <c r="H12" s="17">
+        <v>20</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1</v>
+      </c>
+      <c r="J12" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="L12" s="12">
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="M12" s="17">
         <f>6*6</f>
         <v>36</v>
       </c>
-      <c r="N12" s="12" t="str">
+      <c r="N12" s="12">
         <f t="shared" si="5"/>
-        <v/>
+        <v>36</v>
       </c>
       <c r="O12" s="34" t="s">
         <v>36</v>
@@ -1484,15 +1491,13 @@
       <c r="AU13" s="2"/>
     </row>
     <row r="14" spans="1:47" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
-        <v>1</v>
-      </c>
+      <c r="B14" s="17"/>
       <c r="C14" s="18">
         <v>13.35</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>13.35</v>
+        <v/>
       </c>
       <c r="E14" s="20" t="str">
         <f>HYPERLINK("http://www.digikey.ca/product-detail/en/AD9114BCPZ/AD9114BCPZ-ND","AD9114BCPZ")</f>
@@ -1502,27 +1507,31 @@
         <v>21</v>
       </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="H14" s="17">
+        <v>13</v>
+      </c>
+      <c r="I14" s="17">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L14" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="M14" s="17">
         <f>6*6</f>
         <v>36</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v/>
       </c>
       <c r="O14" s="34" t="s">
         <v>36</v>
@@ -1739,11 +1748,11 @@
       <c r="C18" s="18">
         <v>15.12</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="36">
         <f t="shared" si="1"/>
         <v>15.12</v>
       </c>
-      <c r="E18" s="19" t="str">
+      <c r="E18" s="20" t="str">
         <f>HYPERLINK("http://www.digikey.ca/product-detail/en/AD9288BSTZ-80/AD9288BSTZ-80-ND","AD9288BSTZ-80")</f>
         <v>AD9288BSTZ-80</v>
       </c>
@@ -1874,7 +1883,7 @@
       <c r="C20" s="18">
         <v>19.57</v>
       </c>
-      <c r="D20" s="37" t="str">
+      <c r="D20" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1885,8 +1894,12 @@
       <c r="F20" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="G20" s="17">
+        <v>18</v>
+      </c>
+      <c r="H20" s="17">
+        <v>10</v>
+      </c>
       <c r="J20" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2005,11 +2018,11 @@
       <c r="C22" s="18">
         <v>19.97</v>
       </c>
-      <c r="D22" s="37" t="str">
+      <c r="D22" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E22" s="19" t="str">
+      <c r="E22" s="20" t="str">
         <f>HYPERLINK("http://www.digikey.ca/product-detail/en/LTC2289CUP%23PBF/LTC2289CUP%23PBF-ND","LTC2289CUP#PBF")</f>
         <v>LTC2289CUP#PBF</v>
       </c>
@@ -2232,7 +2245,7 @@
       <c r="C26" s="18">
         <v>7.84</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="36">
         <f t="shared" si="1"/>
         <v>7.84</v>
       </c>
@@ -2244,7 +2257,9 @@
         <v>24</v>
       </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="17">
+        <v>15</v>
+      </c>
       <c r="I26" s="17"/>
       <c r="J26" s="12">
         <f t="shared" si="2"/>
@@ -2252,7 +2267,7 @@
       </c>
       <c r="K26" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L26" s="12">
         <f t="shared" si="4"/>
@@ -2304,7 +2319,7 @@
     <row r="27" spans="1:47" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
-      <c r="D27" s="37" t="str">
+      <c r="D27" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2446,7 +2461,7 @@
       <c r="C31" s="18">
         <v>5.79</v>
       </c>
-      <c r="D31" s="37">
+      <c r="D31" s="36">
         <f t="shared" si="1"/>
         <v>5.79</v>
       </c>
@@ -2456,7 +2471,7 @@
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="12">
+      <c r="I31" s="28">
         <v>16</v>
       </c>
       <c r="J31" s="12">
@@ -2519,6 +2534,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
+      <c r="I32" s="7"/>
       <c r="J32" s="6" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2541,7 +2557,7 @@
       <c r="C33" s="18">
         <v>6.03</v>
       </c>
-      <c r="D33" s="37" t="str">
+      <c r="D33" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2551,7 +2567,7 @@
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="12">
+      <c r="I33" s="28">
         <v>16</v>
       </c>
       <c r="J33" s="12" t="str">
@@ -2714,7 +2730,7 @@
       <c r="C38" s="18">
         <v>7.38</v>
       </c>
-      <c r="D38" s="37" t="str">
+      <c r="D38" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2810,7 +2826,7 @@
       <c r="C40" s="18">
         <v>5.12</v>
       </c>
-      <c r="D40" s="37" t="str">
+      <c r="D40" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2911,7 +2927,7 @@
       <c r="C42" s="18">
         <v>12.67</v>
       </c>
-      <c r="D42" s="37" t="str">
+      <c r="D42" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -3012,7 +3028,7 @@
       <c r="C44" s="18">
         <v>17.48</v>
       </c>
-      <c r="D44" s="37" t="str">
+      <c r="D44" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -3115,7 +3131,7 @@
       <c r="C46" s="18">
         <v>14.92</v>
       </c>
-      <c r="D46" s="37">
+      <c r="D46" s="36">
         <f t="shared" si="1"/>
         <v>14.92</v>
       </c>
@@ -3216,7 +3232,7 @@
       <c r="C48" s="18">
         <v>5.91</v>
       </c>
-      <c r="D48" s="37" t="str">
+      <c r="D48" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -3460,11 +3476,11 @@
       </c>
       <c r="K53" s="6">
         <f t="shared" ref="K53:L53" si="7">SUM(K4:K51)</f>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="L53" s="6">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>38</v>
@@ -3731,7 +3747,7 @@
       </c>
       <c r="D59" s="10">
         <f>SUM(D7:D57)</f>
-        <v>114.60999999999999</v>
+        <v>117.97</v>
       </c>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
@@ -3771,7 +3787,7 @@
       </c>
       <c r="D60" s="10">
         <f>D59*0.13</f>
-        <v>14.899299999999998</v>
+        <v>15.3361</v>
       </c>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -3811,14 +3827,14 @@
       </c>
       <c r="D61" s="9">
         <f>D59+D60</f>
-        <v>129.5093</v>
+        <v>133.30609999999999</v>
       </c>
       <c r="I61" s="6" t="s">
         <v>51</v>
       </c>
       <c r="J61" s="6">
         <f>SUM(J53:L53)</f>
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>

</xml_diff>